<commit_message>
Head Arquivo de Dados ENAs
</commit_message>
<xml_diff>
--- a/ENA_2018_2022.xlsx
+++ b/ENA_2018_2022.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://brookfieldenergia-my.sharepoint.com/personal/anderson_iung_elera_com/Documents/Documentos/00. Pastas e Arquivos antigos/16. Doutorado/00. Material para a Tese/03. Dados/ENAS_2018_2022/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amiun\Desktop\ProjetoGit\Doutorado\Download_Dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1C2F4120-416A-40A1-9EAA-F0BE2BC83AA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6528F63-3859-4F10-B605-6833F1489995}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0F41EF34-B877-4522-A453-96143F9061F4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="3" xr2:uid="{0F41EF34-B877-4522-A453-96143F9061F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sudeste" sheetId="1" r:id="rId1"/>
@@ -39,10 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="4">
-  <si>
-    <t>ENA</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="7">
   <si>
     <t>% MLT</t>
   </si>
@@ -51,6 +48,18 @@
   </si>
   <si>
     <t>Ano</t>
+  </si>
+  <si>
+    <t>ENA_Se</t>
+  </si>
+  <si>
+    <t>ENA_S</t>
+  </si>
+  <si>
+    <t>ENA_Ne</t>
+  </si>
+  <si>
+    <t>ENA_N</t>
   </si>
 </sst>
 </file>
@@ -86,10 +95,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -406,17 +414,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D656422E-8788-4EAC-AC23-5EF6B8A03AEC}">
   <dimension ref="A2:D62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1270,17 +1281,20 @@
   <dimension ref="A2:D62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:D62"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
-        <v>3</v>
+      <c r="C2" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -2133,17 +2147,20 @@
   <dimension ref="A2:D62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:D62"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
-        <v>3</v>
+      <c r="C2" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -2993,10 +3010,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE2B88BF-A595-4CFC-ADF0-10C836FCAE80}">
-  <dimension ref="A1:D62"/>
+  <dimension ref="A2:D62"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3005,24 +3022,18 @@
     <col min="2" max="2" width="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="2"/>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-    </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
       <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
         <v>0</v>
-      </c>
-      <c r="D2" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>